<commit_message>
Update:import work period add
</commit_message>
<xml_diff>
--- a/sample_import.xlsx
+++ b/sample_import.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y23"/>
+  <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -416,17 +416,21 @@
     <col min="12" max="12" width="10.83203125" customWidth="1"/>
     <col min="13" max="13" width="20.83203125" customWidth="1"/>
     <col min="14" max="14" width="6.83203125" customWidth="1"/>
-    <col min="15" max="15" width="18.83203125" customWidth="1"/>
-    <col min="16" max="16" width="12.83203125" customWidth="1"/>
-    <col min="17" max="17" width="12.83203125" customWidth="1"/>
+    <col min="15" max="15" width="10.83203125" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" customWidth="1"/>
+    <col min="17" max="17" width="18.83203125" customWidth="1"/>
     <col min="18" max="18" width="12.83203125" customWidth="1"/>
-    <col min="19" max="19" width="15.83203125" customWidth="1"/>
+    <col min="19" max="19" width="12.83203125" customWidth="1"/>
     <col min="20" max="20" width="14.83203125" customWidth="1"/>
-    <col min="21" max="21" width="12.83203125" customWidth="1"/>
-    <col min="22" max="22" width="14.83203125" customWidth="1"/>
-    <col min="23" max="23" width="10.83203125" customWidth="1"/>
+    <col min="21" max="21" width="14.83203125" customWidth="1"/>
+    <col min="22" max="22" width="12.83203125" customWidth="1"/>
+    <col min="23" max="23" width="15.83203125" customWidth="1"/>
     <col min="24" max="24" width="14.83203125" customWidth="1"/>
-    <col min="25" max="25" width="10.83203125" customWidth="1"/>
+    <col min="25" max="25" width="12.83203125" customWidth="1"/>
+    <col min="26" max="26" width="14.83203125" customWidth="1"/>
+    <col min="27" max="27" width="10.83203125" customWidth="1"/>
+    <col min="28" max="28" width="14.83203125" customWidth="1"/>
+    <col min="29" max="29" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -473,36 +477,48 @@
         <v>부위</v>
       </c>
       <c r="O1" t="str">
+        <v>KLG(우측)</v>
+      </c>
+      <c r="P1" t="str">
+        <v>KLG(좌측)</v>
+      </c>
+      <c r="Q1" t="str">
         <v>직종명</v>
       </c>
-      <c r="P1" t="str">
+      <c r="R1" t="str">
         <v>시작일</v>
       </c>
-      <c r="Q1" t="str">
+      <c r="S1" t="str">
         <v>종료일</v>
       </c>
-      <c r="R1" t="str">
+      <c r="T1" t="str">
+        <v>근무기간(년)</v>
+      </c>
+      <c r="U1" t="str">
+        <v>근무기간(개월)</v>
+      </c>
+      <c r="V1" t="str">
         <v>중량물(kg)</v>
       </c>
-      <c r="S1" t="str">
+      <c r="W1" t="str">
         <v>쪼그려앉기(분)</v>
       </c>
-      <c r="T1" t="str">
+      <c r="X1" t="str">
         <v>계단오르내리기</v>
       </c>
-      <c r="U1" t="str">
+      <c r="Y1" t="str">
         <v>무릎비틀림</v>
       </c>
-      <c r="V1" t="str">
+      <c r="Z1" t="str">
         <v>출발정지반복</v>
       </c>
-      <c r="W1" t="str">
+      <c r="AA1" t="str">
         <v>좁은공간</v>
       </c>
-      <c r="X1" t="str">
+      <c r="AB1" t="str">
         <v>무릎접촉충격</v>
       </c>
-      <c r="Y1" t="str">
+      <c r="AC1" t="str">
         <v>뛰어내리기</v>
       </c>
     </row>
@@ -550,36 +566,48 @@
         <v>우측</v>
       </c>
       <c r="O2" t="str">
+        <v>3</v>
+      </c>
+      <c r="P2" t="str">
+        <v/>
+      </c>
+      <c r="Q2" t="str">
         <v>건설현장 철근공</v>
       </c>
-      <c r="P2" t="str">
+      <c r="R2" t="str">
         <v>1990-03-01</v>
       </c>
-      <c r="Q2" t="str">
+      <c r="S2" t="str">
         <v>2024-01-10</v>
       </c>
-      <c r="R2">
+      <c r="T2">
+        <v>30</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
         <v>2500</v>
       </c>
-      <c r="S2">
+      <c r="W2">
         <v>180</v>
       </c>
-      <c r="T2" t="str">
-        <v>O</v>
-      </c>
-      <c r="U2" t="str">
-        <v>O</v>
-      </c>
-      <c r="V2" t="str">
-        <v/>
-      </c>
-      <c r="W2" t="str">
-        <v/>
-      </c>
       <c r="X2" t="str">
         <v>O</v>
       </c>
       <c r="Y2" t="str">
+        <v>O</v>
+      </c>
+      <c r="Z2" t="str">
+        <v/>
+      </c>
+      <c r="AA2" t="str">
+        <v/>
+      </c>
+      <c r="AB2" t="str">
+        <v>O</v>
+      </c>
+      <c r="AC2" t="str">
         <v>O</v>
       </c>
     </row>
@@ -627,36 +655,48 @@
         <v>양측</v>
       </c>
       <c r="O3" t="str">
+        <v>2</v>
+      </c>
+      <c r="P3" t="str">
+        <v>3</v>
+      </c>
+      <c r="Q3" t="str">
         <v>식당조리사</v>
       </c>
-      <c r="P3" t="str">
+      <c r="R3" t="str">
         <v>1995-06-15</v>
       </c>
-      <c r="Q3" t="str">
+      <c r="S3" t="str">
         <v>2024-02-15</v>
       </c>
-      <c r="R3">
+      <c r="T3" t="str">
+        <v/>
+      </c>
+      <c r="U3" t="str">
+        <v/>
+      </c>
+      <c r="V3">
         <v>500</v>
       </c>
-      <c r="S3">
+      <c r="W3">
         <v>240</v>
       </c>
-      <c r="T3" t="str">
-        <v/>
-      </c>
-      <c r="U3" t="str">
-        <v/>
-      </c>
-      <c r="V3" t="str">
-        <v/>
-      </c>
-      <c r="W3" t="str">
-        <v>O</v>
-      </c>
       <c r="X3" t="str">
         <v/>
       </c>
       <c r="Y3" t="str">
+        <v/>
+      </c>
+      <c r="Z3" t="str">
+        <v/>
+      </c>
+      <c r="AA3" t="str">
+        <v>O</v>
+      </c>
+      <c r="AB3" t="str">
+        <v/>
+      </c>
+      <c r="AC3" t="str">
         <v/>
       </c>
     </row>
@@ -704,36 +744,48 @@
         <v>좌측</v>
       </c>
       <c r="O4" t="str">
+        <v>2</v>
+      </c>
+      <c r="P4" t="str">
+        <v>3</v>
+      </c>
+      <c r="Q4" t="str">
         <v>배관설비공</v>
       </c>
-      <c r="P4" t="str">
+      <c r="R4" t="str">
         <v>1988-04-01</v>
       </c>
-      <c r="Q4" t="str">
+      <c r="S4" t="str">
         <v>2024-03-20</v>
       </c>
-      <c r="R4">
+      <c r="T4" t="str">
+        <v/>
+      </c>
+      <c r="U4" t="str">
+        <v/>
+      </c>
+      <c r="V4">
         <v>1800</v>
       </c>
-      <c r="S4">
+      <c r="W4">
         <v>150</v>
       </c>
-      <c r="T4" t="str">
-        <v>O</v>
-      </c>
-      <c r="U4" t="str">
-        <v/>
-      </c>
-      <c r="V4" t="str">
-        <v>O</v>
-      </c>
-      <c r="W4" t="str">
-        <v>O</v>
-      </c>
       <c r="X4" t="str">
-        <v/>
+        <v>O</v>
       </c>
       <c r="Y4" t="str">
+        <v/>
+      </c>
+      <c r="Z4" t="str">
+        <v>O</v>
+      </c>
+      <c r="AA4" t="str">
+        <v>O</v>
+      </c>
+      <c r="AB4" t="str">
+        <v/>
+      </c>
+      <c r="AC4" t="str">
         <v/>
       </c>
     </row>
@@ -781,36 +833,48 @@
         <v>우측</v>
       </c>
       <c r="O5" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="P5" t="str">
+        <v/>
+      </c>
+      <c r="Q5" t="str">
         <v>청소원</v>
       </c>
-      <c r="P5" t="str">
+      <c r="R5" t="str">
         <v>2000-01-15</v>
       </c>
-      <c r="Q5" t="str">
+      <c r="S5" t="str">
         <v>2024-04-05</v>
       </c>
-      <c r="R5">
+      <c r="T5" t="str">
+        <v/>
+      </c>
+      <c r="U5" t="str">
+        <v/>
+      </c>
+      <c r="V5">
         <v>300</v>
       </c>
-      <c r="S5">
+      <c r="W5">
         <v>200</v>
       </c>
-      <c r="T5" t="str">
-        <v/>
-      </c>
-      <c r="U5" t="str">
-        <v/>
-      </c>
-      <c r="V5" t="str">
-        <v/>
-      </c>
-      <c r="W5" t="str">
-        <v/>
-      </c>
       <c r="X5" t="str">
         <v/>
       </c>
       <c r="Y5" t="str">
+        <v/>
+      </c>
+      <c r="Z5" t="str">
+        <v/>
+      </c>
+      <c r="AA5" t="str">
+        <v/>
+      </c>
+      <c r="AB5" t="str">
+        <v/>
+      </c>
+      <c r="AC5" t="str">
         <v/>
       </c>
     </row>
@@ -858,36 +922,48 @@
         <v>양측</v>
       </c>
       <c r="O6" t="str">
+        <v>4</v>
+      </c>
+      <c r="P6" t="str">
+        <v>3</v>
+      </c>
+      <c r="Q6" t="str">
         <v>택배기사</v>
       </c>
-      <c r="P6" t="str">
+      <c r="R6" t="str">
         <v>1985-07-01</v>
       </c>
-      <c r="Q6" t="str">
+      <c r="S6" t="str">
         <v>2024-05-12</v>
       </c>
-      <c r="R6">
+      <c r="T6" t="str">
+        <v/>
+      </c>
+      <c r="U6" t="str">
+        <v/>
+      </c>
+      <c r="V6">
         <v>2000</v>
       </c>
-      <c r="S6">
+      <c r="W6">
         <v>90</v>
       </c>
-      <c r="T6" t="str">
-        <v>O</v>
-      </c>
-      <c r="U6" t="str">
-        <v/>
-      </c>
-      <c r="V6" t="str">
-        <v>O</v>
-      </c>
-      <c r="W6" t="str">
-        <v/>
-      </c>
       <c r="X6" t="str">
-        <v/>
+        <v>O</v>
       </c>
       <c r="Y6" t="str">
+        <v/>
+      </c>
+      <c r="Z6" t="str">
+        <v>O</v>
+      </c>
+      <c r="AA6" t="str">
+        <v/>
+      </c>
+      <c r="AB6" t="str">
+        <v/>
+      </c>
+      <c r="AC6" t="str">
         <v>O</v>
       </c>
     </row>
@@ -935,36 +1011,48 @@
         <v>좌측</v>
       </c>
       <c r="O7" t="str">
+        <v/>
+      </c>
+      <c r="P7" t="str">
+        <v>2</v>
+      </c>
+      <c r="Q7" t="str">
         <v>간호조무사</v>
       </c>
-      <c r="P7" t="str">
+      <c r="R7" t="str">
         <v>1998-03-01</v>
       </c>
-      <c r="Q7" t="str">
+      <c r="S7" t="str">
         <v>2024-06-18</v>
       </c>
-      <c r="R7">
+      <c r="T7" t="str">
+        <v/>
+      </c>
+      <c r="U7" t="str">
+        <v/>
+      </c>
+      <c r="V7">
         <v>400</v>
       </c>
-      <c r="S7">
+      <c r="W7">
         <v>120</v>
       </c>
-      <c r="T7" t="str">
-        <v/>
-      </c>
-      <c r="U7" t="str">
-        <v>O</v>
-      </c>
-      <c r="V7" t="str">
-        <v/>
-      </c>
-      <c r="W7" t="str">
-        <v/>
-      </c>
       <c r="X7" t="str">
-        <v>O</v>
+        <v/>
       </c>
       <c r="Y7" t="str">
+        <v>O</v>
+      </c>
+      <c r="Z7" t="str">
+        <v/>
+      </c>
+      <c r="AA7" t="str">
+        <v/>
+      </c>
+      <c r="AB7" t="str">
+        <v>O</v>
+      </c>
+      <c r="AC7" t="str">
         <v/>
       </c>
     </row>
@@ -1012,36 +1100,48 @@
         <v>좌측</v>
       </c>
       <c r="O8" t="str">
+        <v/>
+      </c>
+      <c r="P8" t="str">
+        <v>4</v>
+      </c>
+      <c r="Q8" t="str">
         <v>건설현장 철근공</v>
       </c>
-      <c r="P8" t="str">
+      <c r="R8" t="str">
         <v>1990-03-01</v>
       </c>
-      <c r="Q8" t="str">
+      <c r="S8" t="str">
         <v>2024-01-10</v>
       </c>
-      <c r="R8">
+      <c r="T8" t="str">
+        <v/>
+      </c>
+      <c r="U8" t="str">
+        <v/>
+      </c>
+      <c r="V8">
         <v>2500</v>
       </c>
-      <c r="S8">
+      <c r="W8">
         <v>180</v>
       </c>
-      <c r="T8" t="str">
-        <v>O</v>
-      </c>
-      <c r="U8" t="str">
-        <v>O</v>
-      </c>
-      <c r="V8" t="str">
-        <v/>
-      </c>
-      <c r="W8" t="str">
-        <v/>
-      </c>
       <c r="X8" t="str">
         <v>O</v>
       </c>
       <c r="Y8" t="str">
+        <v>O</v>
+      </c>
+      <c r="Z8" t="str">
+        <v/>
+      </c>
+      <c r="AA8" t="str">
+        <v/>
+      </c>
+      <c r="AB8" t="str">
+        <v>O</v>
+      </c>
+      <c r="AC8" t="str">
         <v>O</v>
       </c>
     </row>
@@ -1089,36 +1189,48 @@
         <v>우측</v>
       </c>
       <c r="O9" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="P9" t="str">
+        <v/>
+      </c>
+      <c r="Q9" t="str">
         <v>건설현장 철근공</v>
       </c>
-      <c r="P9" t="str">
+      <c r="R9" t="str">
         <v>1990-03-01</v>
       </c>
-      <c r="Q9" t="str">
+      <c r="S9" t="str">
         <v>2024-01-10</v>
       </c>
-      <c r="R9">
+      <c r="T9" t="str">
+        <v/>
+      </c>
+      <c r="U9" t="str">
+        <v/>
+      </c>
+      <c r="V9">
         <v>2500</v>
       </c>
-      <c r="S9">
+      <c r="W9">
         <v>180</v>
       </c>
-      <c r="T9" t="str">
-        <v>O</v>
-      </c>
-      <c r="U9" t="str">
-        <v>O</v>
-      </c>
-      <c r="V9" t="str">
-        <v/>
-      </c>
-      <c r="W9" t="str">
-        <v/>
-      </c>
       <c r="X9" t="str">
         <v>O</v>
       </c>
       <c r="Y9" t="str">
+        <v>O</v>
+      </c>
+      <c r="Z9" t="str">
+        <v/>
+      </c>
+      <c r="AA9" t="str">
+        <v/>
+      </c>
+      <c r="AB9" t="str">
+        <v>O</v>
+      </c>
+      <c r="AC9" t="str">
         <v>O</v>
       </c>
     </row>
@@ -1166,36 +1278,48 @@
         <v>양측</v>
       </c>
       <c r="O10" t="str">
+        <v/>
+      </c>
+      <c r="P10" t="str">
+        <v/>
+      </c>
+      <c r="Q10" t="str">
         <v>마트 진열원</v>
       </c>
-      <c r="P10" t="str">
+      <c r="R10" t="str">
         <v>2010-01-01</v>
       </c>
-      <c r="Q10" t="str">
+      <c r="S10" t="str">
         <v>2020-12-31</v>
       </c>
-      <c r="R10">
+      <c r="T10" t="str">
+        <v/>
+      </c>
+      <c r="U10" t="str">
+        <v/>
+      </c>
+      <c r="V10">
         <v>800</v>
       </c>
-      <c r="S10">
+      <c r="W10">
         <v>180</v>
       </c>
-      <c r="T10" t="str">
-        <v/>
-      </c>
-      <c r="U10" t="str">
-        <v/>
-      </c>
-      <c r="V10" t="str">
-        <v>O</v>
-      </c>
-      <c r="W10" t="str">
-        <v/>
-      </c>
       <c r="X10" t="str">
         <v/>
       </c>
       <c r="Y10" t="str">
+        <v/>
+      </c>
+      <c r="Z10" t="str">
+        <v>O</v>
+      </c>
+      <c r="AA10" t="str">
+        <v/>
+      </c>
+      <c r="AB10" t="str">
+        <v/>
+      </c>
+      <c r="AC10" t="str">
         <v/>
       </c>
     </row>
@@ -1243,36 +1367,48 @@
         <v>양측</v>
       </c>
       <c r="O11" t="str">
+        <v/>
+      </c>
+      <c r="P11" t="str">
+        <v/>
+      </c>
+      <c r="Q11" t="str">
         <v>공장조립원</v>
       </c>
-      <c r="P11" t="str">
+      <c r="R11" t="str">
         <v>2005-03-01</v>
       </c>
-      <c r="Q11" t="str">
+      <c r="S11" t="str">
         <v>2009-12-31</v>
       </c>
-      <c r="R11">
+      <c r="T11" t="str">
+        <v/>
+      </c>
+      <c r="U11" t="str">
+        <v/>
+      </c>
+      <c r="V11">
         <v>600</v>
       </c>
-      <c r="S11">
+      <c r="W11">
         <v>160</v>
       </c>
-      <c r="T11" t="str">
-        <v/>
-      </c>
-      <c r="U11" t="str">
-        <v>O</v>
-      </c>
-      <c r="V11" t="str">
-        <v>O</v>
-      </c>
-      <c r="W11" t="str">
-        <v/>
-      </c>
       <c r="X11" t="str">
         <v/>
       </c>
       <c r="Y11" t="str">
+        <v>O</v>
+      </c>
+      <c r="Z11" t="str">
+        <v>O</v>
+      </c>
+      <c r="AA11" t="str">
+        <v/>
+      </c>
+      <c r="AB11" t="str">
+        <v/>
+      </c>
+      <c r="AC11" t="str">
         <v/>
       </c>
     </row>
@@ -1320,36 +1456,48 @@
         <v>좌측</v>
       </c>
       <c r="O12" t="str">
+        <v/>
+      </c>
+      <c r="P12" t="str">
+        <v/>
+      </c>
+      <c r="Q12" t="str">
         <v>배관설비공</v>
       </c>
-      <c r="P12" t="str">
+      <c r="R12" t="str">
         <v>1988-04-01</v>
       </c>
-      <c r="Q12" t="str">
+      <c r="S12" t="str">
         <v>2024-03-20</v>
       </c>
-      <c r="R12">
+      <c r="T12" t="str">
+        <v/>
+      </c>
+      <c r="U12" t="str">
+        <v/>
+      </c>
+      <c r="V12">
         <v>1800</v>
       </c>
-      <c r="S12">
+      <c r="W12">
         <v>150</v>
       </c>
-      <c r="T12" t="str">
-        <v>O</v>
-      </c>
-      <c r="U12" t="str">
-        <v/>
-      </c>
-      <c r="V12" t="str">
-        <v>O</v>
-      </c>
-      <c r="W12" t="str">
-        <v>O</v>
-      </c>
       <c r="X12" t="str">
-        <v/>
+        <v>O</v>
       </c>
       <c r="Y12" t="str">
+        <v/>
+      </c>
+      <c r="Z12" t="str">
+        <v>O</v>
+      </c>
+      <c r="AA12" t="str">
+        <v>O</v>
+      </c>
+      <c r="AB12" t="str">
+        <v/>
+      </c>
+      <c r="AC12" t="str">
         <v/>
       </c>
     </row>
@@ -1397,36 +1545,48 @@
         <v>우측</v>
       </c>
       <c r="O13" t="str">
+        <v>2</v>
+      </c>
+      <c r="P13" t="str">
+        <v/>
+      </c>
+      <c r="Q13" t="str">
         <v>미용사</v>
       </c>
-      <c r="P13" t="str">
+      <c r="R13" t="str">
         <v>2003-05-01</v>
       </c>
-      <c r="Q13" t="str">
+      <c r="S13" t="str">
         <v>2024-07-01</v>
       </c>
-      <c r="R13">
+      <c r="T13" t="str">
+        <v/>
+      </c>
+      <c r="U13" t="str">
+        <v/>
+      </c>
+      <c r="V13">
         <v>200</v>
       </c>
-      <c r="S13">
+      <c r="W13">
         <v>300</v>
       </c>
-      <c r="T13" t="str">
-        <v/>
-      </c>
-      <c r="U13" t="str">
-        <v/>
-      </c>
-      <c r="V13" t="str">
-        <v/>
-      </c>
-      <c r="W13" t="str">
-        <v/>
-      </c>
       <c r="X13" t="str">
         <v/>
       </c>
       <c r="Y13" t="str">
+        <v/>
+      </c>
+      <c r="Z13" t="str">
+        <v/>
+      </c>
+      <c r="AA13" t="str">
+        <v/>
+      </c>
+      <c r="AB13" t="str">
+        <v/>
+      </c>
+      <c r="AC13" t="str">
         <v/>
       </c>
     </row>
@@ -1474,36 +1634,48 @@
         <v>양측</v>
       </c>
       <c r="O14" t="str">
+        <v>3</v>
+      </c>
+      <c r="P14" t="str">
+        <v>3</v>
+      </c>
+      <c r="Q14" t="str">
         <v>화물차 운전기사</v>
       </c>
-      <c r="P14" t="str">
+      <c r="R14" t="str">
         <v>1985-01-01</v>
       </c>
-      <c r="Q14" t="str">
+      <c r="S14" t="str">
         <v>2024-08-10</v>
       </c>
-      <c r="R14">
+      <c r="T14">
+        <v>35</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
         <v>1500</v>
       </c>
-      <c r="S14">
+      <c r="W14">
         <v>60</v>
       </c>
-      <c r="T14" t="str">
-        <v/>
-      </c>
-      <c r="U14" t="str">
-        <v/>
-      </c>
-      <c r="V14" t="str">
-        <v>O</v>
-      </c>
-      <c r="W14" t="str">
-        <v/>
-      </c>
       <c r="X14" t="str">
         <v/>
       </c>
       <c r="Y14" t="str">
+        <v/>
+      </c>
+      <c r="Z14" t="str">
+        <v>O</v>
+      </c>
+      <c r="AA14" t="str">
+        <v/>
+      </c>
+      <c r="AB14" t="str">
+        <v/>
+      </c>
+      <c r="AC14" t="str">
         <v>O</v>
       </c>
     </row>
@@ -1551,36 +1723,48 @@
         <v>좌측</v>
       </c>
       <c r="O15" t="str">
+        <v/>
+      </c>
+      <c r="P15" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="Q15" t="str">
         <v>유치원교사</v>
       </c>
-      <c r="P15" t="str">
+      <c r="R15" t="str">
         <v>2005-09-01</v>
       </c>
-      <c r="Q15" t="str">
+      <c r="S15" t="str">
         <v>2024-09-15</v>
       </c>
-      <c r="R15">
+      <c r="T15" t="str">
+        <v/>
+      </c>
+      <c r="U15" t="str">
+        <v/>
+      </c>
+      <c r="V15">
         <v>300</v>
       </c>
-      <c r="S15">
+      <c r="W15">
         <v>250</v>
       </c>
-      <c r="T15" t="str">
-        <v/>
-      </c>
-      <c r="U15" t="str">
-        <v>O</v>
-      </c>
-      <c r="V15" t="str">
-        <v/>
-      </c>
-      <c r="W15" t="str">
-        <v/>
-      </c>
       <c r="X15" t="str">
         <v/>
       </c>
       <c r="Y15" t="str">
+        <v>O</v>
+      </c>
+      <c r="Z15" t="str">
+        <v/>
+      </c>
+      <c r="AA15" t="str">
+        <v/>
+      </c>
+      <c r="AB15" t="str">
+        <v/>
+      </c>
+      <c r="AC15" t="str">
         <v/>
       </c>
     </row>
@@ -1628,36 +1812,48 @@
         <v>양측</v>
       </c>
       <c r="O16" t="str">
+        <v>4</v>
+      </c>
+      <c r="P16" t="str">
+        <v>4</v>
+      </c>
+      <c r="Q16" t="str">
         <v>경비원</v>
       </c>
-      <c r="P16" t="str">
+      <c r="R16" t="str">
         <v>2000-01-01</v>
       </c>
-      <c r="Q16" t="str">
+      <c r="S16" t="str">
         <v>2024-10-20</v>
       </c>
-      <c r="R16">
+      <c r="T16" t="str">
+        <v/>
+      </c>
+      <c r="U16" t="str">
+        <v/>
+      </c>
+      <c r="V16">
         <v>100</v>
       </c>
-      <c r="S16">
+      <c r="W16">
         <v>180</v>
       </c>
-      <c r="T16" t="str">
-        <v>O</v>
-      </c>
-      <c r="U16" t="str">
-        <v/>
-      </c>
-      <c r="V16" t="str">
-        <v/>
-      </c>
-      <c r="W16" t="str">
-        <v/>
-      </c>
       <c r="X16" t="str">
-        <v/>
+        <v>O</v>
       </c>
       <c r="Y16" t="str">
+        <v/>
+      </c>
+      <c r="Z16" t="str">
+        <v/>
+      </c>
+      <c r="AA16" t="str">
+        <v/>
+      </c>
+      <c r="AB16" t="str">
+        <v/>
+      </c>
+      <c r="AC16" t="str">
         <v/>
       </c>
     </row>
@@ -1705,36 +1901,48 @@
         <v>우측</v>
       </c>
       <c r="O17" t="str">
+        <v>1</v>
+      </c>
+      <c r="P17" t="str">
+        <v/>
+      </c>
+      <c r="Q17" t="str">
         <v>공장 품질검사원</v>
       </c>
-      <c r="P17" t="str">
+      <c r="R17" t="str">
         <v>2008-02-01</v>
       </c>
-      <c r="Q17" t="str">
+      <c r="S17" t="str">
         <v>2024-11-05</v>
       </c>
-      <c r="R17">
+      <c r="T17" t="str">
+        <v/>
+      </c>
+      <c r="U17" t="str">
+        <v/>
+      </c>
+      <c r="V17">
         <v>400</v>
       </c>
-      <c r="S17">
+      <c r="W17">
         <v>200</v>
       </c>
-      <c r="T17" t="str">
-        <v/>
-      </c>
-      <c r="U17" t="str">
-        <v/>
-      </c>
-      <c r="V17" t="str">
-        <v>O</v>
-      </c>
-      <c r="W17" t="str">
-        <v>O</v>
-      </c>
       <c r="X17" t="str">
         <v/>
       </c>
       <c r="Y17" t="str">
+        <v/>
+      </c>
+      <c r="Z17" t="str">
+        <v>O</v>
+      </c>
+      <c r="AA17" t="str">
+        <v>O</v>
+      </c>
+      <c r="AB17" t="str">
+        <v/>
+      </c>
+      <c r="AC17" t="str">
         <v/>
       </c>
     </row>
@@ -1782,36 +1990,48 @@
         <v>우측</v>
       </c>
       <c r="O18" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="P18" t="str">
+        <v/>
+      </c>
+      <c r="Q18" t="str">
         <v>농업종사자</v>
       </c>
-      <c r="P18" t="str">
+      <c r="R18" t="str">
         <v>1990-01-01</v>
       </c>
-      <c r="Q18" t="str">
+      <c r="S18" t="str">
         <v>2024-12-01</v>
       </c>
-      <c r="R18">
+      <c r="T18" t="str">
+        <v/>
+      </c>
+      <c r="U18" t="str">
+        <v/>
+      </c>
+      <c r="V18">
         <v>2200</v>
       </c>
-      <c r="S18">
+      <c r="W18">
         <v>280</v>
       </c>
-      <c r="T18" t="str">
-        <v/>
-      </c>
-      <c r="U18" t="str">
-        <v>O</v>
-      </c>
-      <c r="V18" t="str">
-        <v/>
-      </c>
-      <c r="W18" t="str">
-        <v/>
-      </c>
       <c r="X18" t="str">
-        <v>O</v>
+        <v/>
       </c>
       <c r="Y18" t="str">
+        <v>O</v>
+      </c>
+      <c r="Z18" t="str">
+        <v/>
+      </c>
+      <c r="AA18" t="str">
+        <v/>
+      </c>
+      <c r="AB18" t="str">
+        <v>O</v>
+      </c>
+      <c r="AC18" t="str">
         <v/>
       </c>
     </row>
@@ -1859,36 +2079,48 @@
         <v>좌측</v>
       </c>
       <c r="O19" t="str">
+        <v/>
+      </c>
+      <c r="P19" t="str">
+        <v>2</v>
+      </c>
+      <c r="Q19" t="str">
         <v>가사도우미</v>
       </c>
-      <c r="P19" t="str">
+      <c r="R19" t="str">
         <v>1998-06-01</v>
       </c>
-      <c r="Q19" t="str">
+      <c r="S19" t="str">
         <v>2024-12-15</v>
       </c>
-      <c r="R19">
+      <c r="T19" t="str">
+        <v/>
+      </c>
+      <c r="U19" t="str">
+        <v/>
+      </c>
+      <c r="V19">
         <v>350</v>
       </c>
-      <c r="S19">
+      <c r="W19">
         <v>220</v>
       </c>
-      <c r="T19" t="str">
-        <v/>
-      </c>
-      <c r="U19" t="str">
-        <v/>
-      </c>
-      <c r="V19" t="str">
-        <v/>
-      </c>
-      <c r="W19" t="str">
-        <v/>
-      </c>
       <c r="X19" t="str">
         <v/>
       </c>
       <c r="Y19" t="str">
+        <v/>
+      </c>
+      <c r="Z19" t="str">
+        <v/>
+      </c>
+      <c r="AA19" t="str">
+        <v/>
+      </c>
+      <c r="AB19" t="str">
+        <v/>
+      </c>
+      <c r="AC19" t="str">
         <v/>
       </c>
     </row>
@@ -1936,72 +2168,84 @@
         <v>양측</v>
       </c>
       <c r="O20" t="str">
+        <v>3</v>
+      </c>
+      <c r="P20" t="str">
+        <v>2</v>
+      </c>
+      <c r="Q20" t="str">
         <v>제조업 반장</v>
       </c>
-      <c r="P20" t="str">
+      <c r="R20" t="str">
         <v>1980-03-01</v>
       </c>
-      <c r="Q20" t="str">
+      <c r="S20" t="str">
         <v>2025-01-05</v>
       </c>
-      <c r="R20">
+      <c r="T20" t="str">
+        <v/>
+      </c>
+      <c r="U20" t="str">
+        <v/>
+      </c>
+      <c r="V20">
         <v>1800</v>
       </c>
-      <c r="S20">
+      <c r="W20">
         <v>150</v>
       </c>
-      <c r="T20" t="str">
-        <v>O</v>
-      </c>
-      <c r="U20" t="str">
-        <v/>
-      </c>
-      <c r="V20" t="str">
-        <v>O</v>
-      </c>
-      <c r="W20" t="str">
-        <v>O</v>
-      </c>
       <c r="X20" t="str">
-        <v/>
+        <v>O</v>
       </c>
       <c r="Y20" t="str">
+        <v/>
+      </c>
+      <c r="Z20" t="str">
+        <v>O</v>
+      </c>
+      <c r="AA20" t="str">
+        <v>O</v>
+      </c>
+      <c r="AB20" t="str">
+        <v/>
+      </c>
+      <c r="AC20" t="str">
         <v>O</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>홍길동</v>
+        <v>김철수</v>
       </c>
       <c r="B21" t="str">
-        <v>1966-04-10</v>
+        <v>1965-03-15</v>
       </c>
       <c r="C21" t="str">
-        <v>2025-01-10</v>
+        <v>2025-02-01</v>
       </c>
       <c r="D21">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E21">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F21" t="str">
         <v>남</v>
       </c>
       <c r="G21" t="str">
-        <v>세종병원</v>
+        <v>서울대병원</v>
       </c>
       <c r="H21" t="str">
         <v>정형외과</v>
       </c>
       <c r="I21" t="str">
-        <v>권의사</v>
+        <v>이의사</v>
       </c>
       <c r="J21" t="str">
-        <v>양쪽 무릎 모두 심함</v>
+        <v>재발</v>
       </c>
       <c r="K21" t="str">
-        <v>휠체어 사용 권고</v>
+        <v/>
       </c>
       <c r="L21" t="str">
         <v>M17.1</v>
@@ -2013,69 +2257,81 @@
         <v>우측</v>
       </c>
       <c r="O21" t="str">
-        <v>타일공</v>
+        <v>3</v>
       </c>
       <c r="P21" t="str">
-        <v>1988-01-01</v>
+        <v/>
       </c>
       <c r="Q21" t="str">
-        <v>2020-12-31</v>
-      </c>
-      <c r="R21">
-        <v>2800</v>
-      </c>
-      <c r="S21">
-        <v>320</v>
+        <v>건설현장 철근공</v>
+      </c>
+      <c r="R21" t="str">
+        <v>1990-03-01</v>
+      </c>
+      <c r="S21" t="str">
+        <v>2025-02-01</v>
       </c>
       <c r="T21" t="str">
-        <v>O</v>
+        <v/>
       </c>
       <c r="U21" t="str">
-        <v>O</v>
-      </c>
-      <c r="V21" t="str">
-        <v>O</v>
-      </c>
-      <c r="W21" t="str">
-        <v>O</v>
+        <v/>
+      </c>
+      <c r="V21">
+        <v>2500</v>
+      </c>
+      <c r="W21">
+        <v>180</v>
       </c>
       <c r="X21" t="str">
         <v>O</v>
       </c>
       <c r="Y21" t="str">
+        <v>O</v>
+      </c>
+      <c r="Z21" t="str">
+        <v/>
+      </c>
+      <c r="AA21" t="str">
+        <v/>
+      </c>
+      <c r="AB21" t="str">
+        <v>O</v>
+      </c>
+      <c r="AC21" t="str">
         <v>O</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>홍길동</v>
+        <v>이영희</v>
       </c>
       <c r="B22" t="str">
-        <v>1966-04-10</v>
+        <v>1970-08-22</v>
       </c>
       <c r="C22" t="str">
-        <v>2025-01-10</v>
+        <v>2025-03-10</v>
       </c>
       <c r="D22">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="E22">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F22" t="str">
-        <v>남</v>
+        <v>여</v>
       </c>
       <c r="G22" t="str">
-        <v>세종병원</v>
+        <v>연세세브란스</v>
       </c>
       <c r="H22" t="str">
-        <v>정형외과</v>
+        <v>재활의학과</v>
       </c>
       <c r="I22" t="str">
-        <v>권의사</v>
+        <v>박의사</v>
       </c>
       <c r="J22" t="str">
-        <v/>
+        <v>재발</v>
       </c>
       <c r="K22" t="str">
         <v/>
@@ -2087,40 +2343,52 @@
         <v>일차성 무릎관절증</v>
       </c>
       <c r="N22" t="str">
-        <v>좌측</v>
+        <v>양측</v>
       </c>
       <c r="O22" t="str">
-        <v>타일공</v>
+        <v>2</v>
       </c>
       <c r="P22" t="str">
-        <v>1988-01-01</v>
+        <v>3</v>
       </c>
       <c r="Q22" t="str">
-        <v>2020-12-31</v>
-      </c>
-      <c r="R22">
-        <v>2800</v>
-      </c>
-      <c r="S22">
-        <v>320</v>
+        <v>식당조리사</v>
+      </c>
+      <c r="R22" t="str">
+        <v>1995-06-15</v>
+      </c>
+      <c r="S22" t="str">
+        <v>2025-03-10</v>
       </c>
       <c r="T22" t="str">
-        <v>O</v>
+        <v/>
       </c>
       <c r="U22" t="str">
-        <v>O</v>
-      </c>
-      <c r="V22" t="str">
-        <v>O</v>
-      </c>
-      <c r="W22" t="str">
-        <v>O</v>
+        <v/>
+      </c>
+      <c r="V22">
+        <v>500</v>
+      </c>
+      <c r="W22">
+        <v>240</v>
       </c>
       <c r="X22" t="str">
-        <v>O</v>
+        <v/>
       </c>
       <c r="Y22" t="str">
-        <v>O</v>
+        <v/>
+      </c>
+      <c r="Z22" t="str">
+        <v/>
+      </c>
+      <c r="AA22" t="str">
+        <v>O</v>
+      </c>
+      <c r="AB22" t="str">
+        <v/>
+      </c>
+      <c r="AC22" t="str">
+        <v/>
       </c>
     </row>
     <row r="23">
@@ -2152,57 +2420,247 @@
         <v>권의사</v>
       </c>
       <c r="J23" t="str">
-        <v/>
+        <v>양쪽 무릎 모두 심함</v>
       </c>
       <c r="K23" t="str">
-        <v/>
+        <v>휠체어 사용 권고</v>
       </c>
       <c r="L23" t="str">
-        <v>M23.2</v>
+        <v>M17.1</v>
       </c>
       <c r="M23" t="str">
-        <v>반월상연골손상</v>
+        <v>일차성 무릎관절증</v>
       </c>
       <c r="N23" t="str">
         <v>우측</v>
       </c>
       <c r="O23" t="str">
+        <v>4</v>
+      </c>
+      <c r="P23" t="str">
+        <v/>
+      </c>
+      <c r="Q23" t="str">
+        <v>타일공</v>
+      </c>
+      <c r="R23" t="str">
+        <v>1988-01-01</v>
+      </c>
+      <c r="S23" t="str">
+        <v>2020-12-31</v>
+      </c>
+      <c r="T23" t="str">
+        <v/>
+      </c>
+      <c r="U23" t="str">
+        <v/>
+      </c>
+      <c r="V23">
+        <v>2800</v>
+      </c>
+      <c r="W23">
+        <v>320</v>
+      </c>
+      <c r="X23" t="str">
+        <v>O</v>
+      </c>
+      <c r="Y23" t="str">
+        <v>O</v>
+      </c>
+      <c r="Z23" t="str">
+        <v>O</v>
+      </c>
+      <c r="AA23" t="str">
+        <v>O</v>
+      </c>
+      <c r="AB23" t="str">
+        <v>O</v>
+      </c>
+      <c r="AC23" t="str">
+        <v>O</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>홍길동</v>
+      </c>
+      <c r="B24" t="str">
+        <v>1966-04-10</v>
+      </c>
+      <c r="C24" t="str">
+        <v>2025-01-10</v>
+      </c>
+      <c r="D24">
+        <v>171</v>
+      </c>
+      <c r="E24">
+        <v>72</v>
+      </c>
+      <c r="F24" t="str">
+        <v>남</v>
+      </c>
+      <c r="G24" t="str">
+        <v>세종병원</v>
+      </c>
+      <c r="H24" t="str">
+        <v>정형외과</v>
+      </c>
+      <c r="I24" t="str">
+        <v>권의사</v>
+      </c>
+      <c r="J24" t="str">
+        <v/>
+      </c>
+      <c r="K24" t="str">
+        <v/>
+      </c>
+      <c r="L24" t="str">
+        <v>M17.1</v>
+      </c>
+      <c r="M24" t="str">
+        <v>일차성 무릎관절증</v>
+      </c>
+      <c r="N24" t="str">
+        <v>좌측</v>
+      </c>
+      <c r="O24" t="str">
+        <v/>
+      </c>
+      <c r="P24" t="str">
+        <v>3</v>
+      </c>
+      <c r="Q24" t="str">
+        <v>타일공</v>
+      </c>
+      <c r="R24" t="str">
+        <v>1988-01-01</v>
+      </c>
+      <c r="S24" t="str">
+        <v>2020-12-31</v>
+      </c>
+      <c r="T24" t="str">
+        <v/>
+      </c>
+      <c r="U24" t="str">
+        <v/>
+      </c>
+      <c r="V24">
+        <v>2800</v>
+      </c>
+      <c r="W24">
+        <v>320</v>
+      </c>
+      <c r="X24" t="str">
+        <v>O</v>
+      </c>
+      <c r="Y24" t="str">
+        <v>O</v>
+      </c>
+      <c r="Z24" t="str">
+        <v>O</v>
+      </c>
+      <c r="AA24" t="str">
+        <v>O</v>
+      </c>
+      <c r="AB24" t="str">
+        <v>O</v>
+      </c>
+      <c r="AC24" t="str">
+        <v>O</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>홍길동</v>
+      </c>
+      <c r="B25" t="str">
+        <v>1966-04-10</v>
+      </c>
+      <c r="C25" t="str">
+        <v>2025-01-10</v>
+      </c>
+      <c r="D25">
+        <v>171</v>
+      </c>
+      <c r="E25">
+        <v>72</v>
+      </c>
+      <c r="F25" t="str">
+        <v>남</v>
+      </c>
+      <c r="G25" t="str">
+        <v>세종병원</v>
+      </c>
+      <c r="H25" t="str">
+        <v>정형외과</v>
+      </c>
+      <c r="I25" t="str">
+        <v>권의사</v>
+      </c>
+      <c r="J25" t="str">
+        <v/>
+      </c>
+      <c r="K25" t="str">
+        <v/>
+      </c>
+      <c r="L25" t="str">
+        <v>M23.2</v>
+      </c>
+      <c r="M25" t="str">
+        <v>반월상연골손상</v>
+      </c>
+      <c r="N25" t="str">
+        <v>우측</v>
+      </c>
+      <c r="O25" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="P25" t="str">
+        <v/>
+      </c>
+      <c r="Q25" t="str">
         <v>미장공</v>
       </c>
-      <c r="P23" t="str">
+      <c r="R25" t="str">
         <v>2021-01-01</v>
       </c>
-      <c r="Q23" t="str">
+      <c r="S25" t="str">
         <v>2025-01-10</v>
       </c>
-      <c r="R23">
+      <c r="T25" t="str">
+        <v/>
+      </c>
+      <c r="U25" t="str">
+        <v/>
+      </c>
+      <c r="V25">
         <v>2000</v>
       </c>
-      <c r="S23">
+      <c r="W25">
         <v>250</v>
       </c>
-      <c r="T23" t="str">
-        <v>O</v>
-      </c>
-      <c r="U23" t="str">
-        <v>O</v>
-      </c>
-      <c r="V23" t="str">
-        <v/>
-      </c>
-      <c r="W23" t="str">
-        <v>O</v>
-      </c>
-      <c r="X23" t="str">
-        <v/>
-      </c>
-      <c r="Y23" t="str">
+      <c r="X25" t="str">
+        <v>O</v>
+      </c>
+      <c r="Y25" t="str">
+        <v>O</v>
+      </c>
+      <c r="Z25" t="str">
+        <v/>
+      </c>
+      <c r="AA25" t="str">
+        <v>O</v>
+      </c>
+      <c r="AB25" t="str">
+        <v/>
+      </c>
+      <c r="AC25" t="str">
         <v>O</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:Y23"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AC25"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>